<commit_message>
ajuste en el login
</commit_message>
<xml_diff>
--- a/Servicios Villa Campestre.xlsx
+++ b/Servicios Villa Campestre.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cristian.lopera/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/villa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DDEA02-EC31-254A-89B3-5FCB200CDE55}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8558F0D-5687-D249-A736-FCE733580A88}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8259CFA5-B4FB-5E45-978E-DD00EB305BB7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{8259CFA5-B4FB-5E45-978E-DD00EB305BB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={1A7077E6-D0EB-0747-9851-3832696FC62A}</author>
+    <author>tc={9FA73004-6F9F-F44D-AF40-0BB20CE2F916}</author>
   </authors>
   <commentList>
     <comment ref="C5" authorId="0" shapeId="0" xr:uid="{1A7077E6-D0EB-0747-9851-3832696FC62A}">
@@ -42,6 +43,15 @@
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     columnDBSearch es el nombre de  la columna en la tabla usuario por la que se va a buscar</t>
+      </text>
+    </comment>
+    <comment ref="D6" authorId="1" shapeId="0" xr:uid="{9FA73004-6F9F-F44D-AF40-0BB20CE2F916}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Los valores que pueden llegar en  rol son:
+ADMIN,SECRET,EMPLOYEE</t>
       </text>
     </comment>
   </commentList>
@@ -193,18 +203,6 @@
     <t>Login</t>
   </si>
   <si>
-    <t>{
-    "status": "error",
-    "message": "Contraseña incorrecta."
-}</t>
-  </si>
-  <si>
-    <t>{
-    "status": "success",
-    "message": "sesion iniciada."
-}</t>
-  </si>
-  <si>
     <t>Finalizar sesion</t>
   </si>
   <si>
@@ -220,6 +218,20 @@
     <t>{
     "status": "success",
     "message": "sesion finalizada."
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "success",
+    "message": "Contraseña incorrecta.",
+    "rol" : "tipo_rol"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": "Contraseña incorrecta.",
+    "rol" : null
 }</t>
   </si>
 </sst>
@@ -527,17 +539,47 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
+    </dxf>
+    <dxf>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -559,36 +601,6 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -611,10 +623,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DC0E40D0-175E-A043-B700-52DCB96B4C6A}" name="Tabla1" displayName="Tabla1" ref="A1:E16" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DC0E40D0-175E-A043-B700-52DCB96B4C6A}" name="Tabla1" displayName="Tabla1" ref="A1:E16" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <autoFilter ref="A1:E16" xr:uid="{F36B9FEE-7844-BB45-951C-914229BB8FBD}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6F49297A-0900-E14B-83B2-2AE43C037C74}" name="SERVICIO" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{6F49297A-0900-E14B-83B2-2AE43C037C74}" name="SERVICIO" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{57EE9C9E-ADBE-BC4F-AB61-34182D5C23CF}" name="URL" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{B01C19D5-1B37-9548-B550-43BC8336EB9E}" name="REQUEST" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{256E2A0D-5A90-444B-AF02-39076F07DA18}" name="RESPONSE SUCCESS" dataDxfId="1"/>
@@ -924,6 +936,10 @@
   <threadedComment ref="C5" dT="2019-09-05T20:07:56.70" personId="{09DFB343-EC5A-084B-9E0D-3C8610716132}" id="{1A7077E6-D0EB-0747-9851-3832696FC62A}">
     <text>columnDBSearch es el nombre de  la columna en la tabla usuario por la que se va a buscar</text>
   </threadedComment>
+  <threadedComment ref="D6" dT="2019-09-07T20:08:08.95" personId="{09DFB343-EC5A-084B-9E0D-3C8610716132}" id="{9FA73004-6F9F-F44D-AF40-0BB20CE2F916}">
+    <text>Los valores que pueden llegar en  rol son:
+ADMIN,SECRET,EMPLOYEE</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -931,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F7EBD3-0618-2440-AF04-A7ADAD9C114C}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1029,7 +1045,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="68">
+    <row r="6" spans="1:5" ht="85">
       <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
@@ -1040,27 +1056,27 @@
         <v>23</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="68">
       <c r="A7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="D7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>29</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:5">

</xml_diff>

<commit_message>
DB y algo de reservas
</commit_message>
<xml_diff>
--- a/Servicios Villa Campestre.xlsx
+++ b/Servicios Villa Campestre.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/villa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3F2706-E855-E842-8D3D-22FAB3A2AB16}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553D8A44-A161-2848-8EA1-A0F5D3A3298F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{8259CFA5-B4FB-5E45-978E-DD00EB305BB7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8259CFA5-B4FB-5E45-978E-DD00EB305BB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,7 @@
     <author>tc={9FA73004-6F9F-F44D-AF40-0BB20CE2F916}</author>
     <author>tc={D6EDB8B0-3E95-AA42-B896-2BD89CE112DB}</author>
     <author>tc={534F4A33-E0AE-2442-A728-6FAC016281EF}</author>
+    <author>tc={1DDB269C-1014-8646-BD6C-312232272698}</author>
   </authors>
   <commentList>
     <comment ref="C6" authorId="0" shapeId="0" xr:uid="{1A7077E6-D0EB-0747-9851-3832696FC62A}">
@@ -74,12 +75,20 @@
     En la imagen  valida lo mismo que valida en el servicio de  modificar producto</t>
       </text>
     </comment>
+    <comment ref="D43" authorId="4" shapeId="0" xr:uid="{1DDB269C-1014-8646-BD6C-312232272698}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    promocion y productos  llegan NULL cuando no es promocion o no  hay productos</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="191">
   <si>
     <t>SERVICIO</t>
   </si>
@@ -416,26 +425,6 @@
     <t>{
     "columnDBSearch": "1",
     "value": "1"
-}</t>
-  </si>
-  <si>
-    <t>{
-    "status": "success",
-    "message": "Consultas realizada.",
-    "data": [
-        {
-            "hab_numero": "2",
-            "id_tipo_habitacion": "1",
-            "hab_detalle": "",
-            "hab_fecha_creacion": "2019-09-08",
-            "hab_estado": "1",
-            "th_nombre_tipo": "Premium",
-            "th_descripcion": "Cama doble para tiki tiki",
-            "th_valor_hora": "20000",
-            "th_valor_persona_adicional": "12000",
-            "th_estado": "1",
-            "th_fecha_creacion": "2019-09-07"
-        }      ]
 }</t>
   </si>
   <si>
@@ -1041,12 +1030,207 @@
     "valor_inicial":"20000"
 }</t>
   </si>
+  <si>
+    <t>{
+    "status": "success",
+    "message": "Consultas realizada.",
+    "data": [
+        {
+            "hab_numero": "1",
+            "hab_detalle": "nada",
+            "sr_estado_reserva": "2",
+            "hab_estado": "1",
+            "th_nombre_tipo": "Premium",
+            "th_valor_hora": "20000",
+            "th_valor_persona_adicional": "12000",
+            "sr_nombre": "Reservada",
+            "sr_color": "#000",
+            "tiempo_transcurido": "16:54:00"
+        },
+        {
+            "hab_numero": "2",
+            "hab_detalle": "",
+            "sr_estado_reserva": "1",
+            "hab_estado": "1",
+            "th_nombre_tipo": "Premium",
+            "th_valor_hora": "20000",
+            "th_valor_persona_adicional": "12000",
+            "sr_nombre": "Disponible",
+            "sr_color": "#fff"
+        }
+    ]
+}</t>
+  </si>
+  <si>
+    <t>CrearReserva</t>
+  </si>
+  <si>
+    <t>Crear Reserva</t>
+  </si>
+  <si>
+    <t>{
+    "hab_numero": "1",
+    "promocion": "",
+    "tipo_reserva": "2",
+    "numero_personas_adicionales": "0",
+    "habitacion_decorada": "1",
+    "productos": [
+            {"id":8,"cantidad":1},
+            {"id":9,"cantidad":5}
+        ]
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": "Esta habitación ya se encuentra reservada."
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "success",
+    "message": "Reserva creada exitosamente."
+}</t>
+  </si>
+  <si>
+    <t>ModificarReserva</t>
+  </si>
+  <si>
+    <t>Moficar reserva</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": "Esta habitación no se encuentra reservada."
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "success",
+    "message": "Reserva modificada exitosamente."
+}</t>
+  </si>
+  <si>
+    <t>{
+    "id_reserva": "38",
+    "numero_personas_adicionales": "1",
+    "habitacion_decorada": "1",
+    "productos": [
+        {"id":8,"cantidad":1},
+        {"id":9,"cantidad":5},
+        {"id":12,"cantidad":10}
+        ]
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detalles de la reserva </t>
+  </si>
+  <si>
+    <t>detallesReserva</t>
+  </si>
+  <si>
+    <t>{
+    "habitacion":"1"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "success",
+    "message": "Consultas realizada.",
+    "data": {
+        "reserva": {
+            "hab_numero": "2",
+            "id_tipo_habitacion": "1",
+            "hab_detalle": "",
+            "sr_estado_reserva": "2",
+            "hab_fecha_creacion": "2019-09-08",
+            "hab_estado": "1",
+            "sr_nombre": "Reservada",
+            "sr_descripcion": "",
+            "sr_color": "#000",
+            "th_nombre_tipo": "Premium",
+            "th_descripcion": "Cama doble para tiki tiki",
+            "th_valor_hora": "20000",
+            "th_valor_persona_adicional": "12000",
+            "th_estado": "1",
+            "th_fecha_creacion": "2019-09-07",
+            "id_reserva": "39",
+            "id_usuario": "6",
+            "promo_id": "1",
+            "ra_fecha_hora_ingreso": "2019-09-16 14:13:10",
+            "ra_inicio_tiempo_parcial": null,
+            "ra_fin_tiempo_parcial": null,
+            "ra_numero_personas_adicionales": "1",
+            "ra_habitacion_decorada": "1"
+        },
+        "productos": [
+            {
+                "id_detalle": "131",
+                "id_reserva": "39",
+                "re_det_id_producto": "8",
+                "re_det_cantidad": "1",
+                "re_precio_compra": "19000",
+                "re_det_valor_unidad": "20000",
+                "re_det_valor_total": "20000"
+            },
+            {
+                "id_detalle": "132",
+                "id_reserva": "39",
+                "re_det_id_producto": "9",
+                "re_det_cantidad": "5",
+                "re_precio_compra": "19000",
+                "re_det_valor_unidad": "20000",
+                "re_det_valor_total": "100000"
+            }
+        ]
+    },
+    "promocion": {
+        "id_promocion": "1",
+        "promo_tiempo": "04:00:00",
+        "promo_valor": "30000",
+        "promo_fecha_registro": "2019-09-05",
+        "id_usuario": "6"
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": "no hay información asociada a esta consulta verifica si la habitación esta reservada.",
+    "data": null,
+    "promocion": null
+}</t>
+  </si>
+  <si>
+    <t>Cambiar estado reserva</t>
+  </si>
+  <si>
+    <t>cambiarEstadoReserva</t>
+  </si>
+  <si>
+    <t>{
+    "habitacion":3,
+    "estado_reserva",3
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "success",
+    "message": "Tiempo parcial Finalizado"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": "Este estado de reserva no existe en nuestro sistema."
+}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1081,6 +1265,12 @@
       <sz val="12"/>
       <color rgb="FF505050"/>
       <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1755,6 +1945,9 @@
   <threadedComment ref="C34" dT="2019-09-12T21:21:02.95" personId="{09DFB343-EC5A-084B-9E0D-3C8610716132}" id="{534F4A33-E0AE-2442-A728-6FAC016281EF}">
     <text>En la imagen  valida lo mismo que valida en el servicio de  modificar producto</text>
   </threadedComment>
+  <threadedComment ref="D43" dT="2019-09-16T19:15:37.57" personId="{09DFB343-EC5A-084B-9E0D-3C8610716132}" id="{1DDB269C-1014-8646-BD6C-312232272698}">
+    <text>promocion y productos  llegan NULL cuando no es promocion o no  hay productos</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1762,8 +1955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F7EBD3-0618-2440-AF04-A7ADAD9C114C}">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1845,16 +2038,16 @@
     </row>
     <row r="5" spans="1:5" ht="119">
       <c r="A5" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>152</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>153</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>52</v>
@@ -2013,7 +2206,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="306">
+    <row r="15" spans="1:5" ht="409.6">
       <c r="A15" s="4" t="s">
         <v>61</v>
       </c>
@@ -2024,7 +2217,7 @@
         <v>63</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>64</v>
+        <v>170</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>52</v>
@@ -2032,16 +2225,16 @@
     </row>
     <row r="16" spans="1:5" ht="119">
       <c r="A16" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>155</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>156</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>52</v>
@@ -2049,101 +2242,101 @@
     </row>
     <row r="17" spans="1:5" ht="102">
       <c r="A17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="C17" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="D17" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="E17" s="10" t="s">
         <v>68</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="85">
       <c r="A18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="D18" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" s="18" t="s">
+      <c r="E18" s="20" t="s">
         <v>73</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="204">
       <c r="A19" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="C19" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D19" s="8" t="s">
+      <c r="E19" s="10" t="s">
         <v>77</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="221">
       <c r="A20" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="C20" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="10" t="s">
         <v>80</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="85">
       <c r="A21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="15" t="s">
         <v>83</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>84</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>45</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="340">
       <c r="A22" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="15" t="s">
         <v>87</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>88</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>63</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>52</v>
@@ -2151,67 +2344,67 @@
     </row>
     <row r="23" spans="1:5" ht="85">
       <c r="A23" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="C23" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" s="10" t="s">
         <v>91</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="102">
       <c r="A24" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B24" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" s="10" t="s">
         <v>97</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="85">
       <c r="A25" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C25" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" s="10" t="s">
         <v>101</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="221">
       <c r="A26" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="19" t="s">
         <v>105</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>106</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>63</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E26" s="20" t="s">
         <v>52</v>
@@ -2219,67 +2412,67 @@
     </row>
     <row r="27" spans="1:5" ht="170">
       <c r="A27" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E27" s="20" t="s">
         <v>109</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="E27" s="20" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="204">
       <c r="A28" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="E28" s="20" t="s">
         <v>115</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E28" s="20" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="85">
       <c r="A29" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="C29" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E29" s="20" t="s">
         <v>118</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="119">
       <c r="A30" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B30" s="15" t="s">
         <v>149</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>150</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>27</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E30" s="10" t="s">
         <v>52</v>
@@ -2287,16 +2480,16 @@
     </row>
     <row r="31" spans="1:5" ht="340">
       <c r="A31" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" s="15" t="s">
         <v>121</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>122</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>63</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E31" s="20" t="s">
         <v>52</v>
@@ -2304,33 +2497,33 @@
     </row>
     <row r="32" spans="1:5" ht="102">
       <c r="A32" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="C32" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="E32" s="20" t="s">
         <v>127</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="E32" s="20" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="204">
       <c r="A33" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" s="15" t="s">
         <v>129</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>130</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>63</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E33" s="20" t="s">
         <v>52</v>
@@ -2338,33 +2531,33 @@
     </row>
     <row r="34" spans="1:5" ht="340">
       <c r="A34" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="C34" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="E34" s="20" t="s">
         <v>135</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="E34" s="20" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="409.6">
       <c r="A35" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E35" s="20" t="s">
         <v>52</v>
@@ -2372,33 +2565,33 @@
     </row>
     <row r="36" spans="1:5" ht="85">
       <c r="A36" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B36" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="C36" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="D36" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E36" s="20" t="s">
         <v>144</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="E36" s="20" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="170">
       <c r="A37" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E37" s="20" t="s">
         <v>52</v>
@@ -2406,82 +2599,122 @@
     </row>
     <row r="38" spans="1:5" ht="85">
       <c r="A38" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="B38" s="15" t="s">
         <v>158</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>159</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E38" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="85">
       <c r="A39" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B39" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="C39" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E39" s="20" t="s">
         <v>163</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="E39" s="20" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="85">
       <c r="A40" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B40" s="15" t="s">
         <v>166</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>167</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>27</v>
       </c>
       <c r="D40" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="E40" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="E40" s="20" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="4"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="12"/>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="4"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="12"/>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="4"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="12"/>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="4"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="12"/>
+    </row>
+    <row r="41" spans="1:5" ht="187">
+      <c r="A41" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="170">
+      <c r="A42" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="409.6">
+      <c r="A43" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="85">
+      <c r="A44" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="E44" s="20" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="4"/>

</xml_diff>